<commit_message>
add JC updated evidence tables
</commit_message>
<xml_diff>
--- a/data/raw/Attribute-Weights.xlsx
+++ b/data/raw/Attribute-Weights.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIIVIAK\Dropbox\0. PhD documents\Performance Matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross Wilson\GitHub Projects\CMOR-evidence-table\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C333534A-7EB3-4809-830E-252AFAC01DFB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7910" windowHeight="3660" xr2:uid="{D24AC9A7-2B13-4C0B-9541-EE128E001DD8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7905" windowHeight="3660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +65,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,19 +126,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,31 +453,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2998781F-954E-499B-91FE-1800D39C8FF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>1</v>
@@ -492,7 +495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -506,7 +509,7 @@
         <v>6.2685000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -520,7 +523,7 @@
         <v>9.4110999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -534,7 +537,7 @@
         <v>12.8225</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -548,7 +551,7 @@
         <v>15.010300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -568,21 +571,24 @@
         <v>19.0487</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
+        <v>3.7415500000000002</v>
+      </c>
+      <c r="D8">
         <v>7.4831000000000003</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>13.182399999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -596,7 +602,7 @@
         <v>6.6089000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
update to final (!) version of RACGP evidence table
</commit_message>
<xml_diff>
--- a/data/raw/Attribute-Weights.xlsx
+++ b/data/raw/Attribute-Weights.xlsx
@@ -133,13 +133,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,13 +469,13 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -506,7 +506,7 @@
         <v>3.1339999999999999</v>
       </c>
       <c r="D3">
-        <v>6.2685000000000004</v>
+        <v>6.2685227799999996</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -517,10 +517,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5.2743000000000002</v>
+        <v>5.2743417990000001</v>
       </c>
       <c r="D4">
-        <v>9.4110999999999994</v>
+        <v>9.4110842520000002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -531,10 +531,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>7.9470000000000001</v>
+        <v>7.9470410280000001</v>
       </c>
       <c r="D5">
-        <v>12.8225</v>
+        <v>12.822451210000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -545,10 +545,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>9.8308999999999997</v>
+        <v>9.8308525109999998</v>
       </c>
       <c r="D6">
-        <v>15.010300000000001</v>
+        <v>15.010274730000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,16 +559,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>6.4672999999999998</v>
+        <v>6.4672902390000004</v>
       </c>
       <c r="D7">
         <v>11.084</v>
       </c>
       <c r="E7">
-        <v>15.2942</v>
+        <v>15.294215489999999</v>
       </c>
       <c r="F7">
-        <v>19.0487</v>
+        <v>19.048720880000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -578,14 +578,14 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="6">
-        <v>3.7415500000000002</v>
+      <c r="C8" s="4">
+        <v>3.923</v>
       </c>
       <c r="D8">
-        <v>7.4831000000000003</v>
+        <v>7.4831314799999999</v>
       </c>
       <c r="E8">
-        <v>13.182399999999999</v>
+        <v>13.182373630000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>4.0721999999999996</v>
+        <v>4.0721779700000003</v>
       </c>
       <c r="D9">
-        <v>6.6089000000000002</v>
+        <v>6.6089478929999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -610,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>5.8734000000000002</v>
+        <v>5.8733768309999999</v>
       </c>
       <c r="D10" s="1">
-        <v>13.1914</v>
+        <v>13.191412809999999</v>
       </c>
       <c r="E10" s="1">
-        <v>17.647600000000001</v>
+        <v>17.647624629999999</v>
       </c>
       <c r="F10" s="1"/>
     </row>

</xml_diff>